<commit_message>
Branch Perfil Empleados Multi-Clientes
</commit_message>
<xml_diff>
--- a/Documentos/Análisis/Selección Múltiple de Clientes en Perfil de Empleados.xlsx
+++ b/Documentos/Análisis/Selección Múltiple de Clientes en Perfil de Empleados.xlsx
@@ -263,11 +263,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -284,13 +285,26 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -327,8 +341,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -360,7 +378,7 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C65" activeCellId="0" sqref="C65"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -383,10 +401,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -411,7 +429,7 @@
       <c r="B4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -422,7 +440,7 @@
       <c r="B5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -433,7 +451,7 @@
       <c r="B6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -441,10 +459,10 @@
       <c r="A7" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -452,10 +470,10 @@
       <c r="A8" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -463,10 +481,10 @@
       <c r="A9" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -477,7 +495,7 @@
       <c r="B10" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -485,7 +503,7 @@
       <c r="B11" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -493,7 +511,7 @@
       <c r="B12" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -501,7 +519,7 @@
       <c r="B13" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -509,7 +527,7 @@
       <c r="B14" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -517,10 +535,10 @@
       <c r="A15" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -531,7 +549,7 @@
       <c r="B16" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -539,7 +557,7 @@
       <c r="B17" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -547,7 +565,7 @@
       <c r="B18" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -558,7 +576,7 @@
       <c r="B19" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -566,7 +584,7 @@
       <c r="B20" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -574,7 +592,7 @@
       <c r="B21" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -585,7 +603,7 @@
       <c r="B22" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -593,7 +611,7 @@
       <c r="B23" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -604,7 +622,7 @@
       <c r="B24" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -615,7 +633,7 @@
       <c r="B25" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -623,7 +641,7 @@
       <c r="B26" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -631,7 +649,7 @@
       <c r="B27" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -639,10 +657,10 @@
       <c r="A28" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" s="1" t="s">
+      <c r="B28" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -672,10 +690,10 @@
       <c r="A31" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="B31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -683,10 +701,10 @@
       <c r="A32" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="1" t="s">
+      <c r="B32" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -694,10 +712,10 @@
       <c r="A33" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" s="1" t="s">
+      <c r="B33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -716,10 +734,10 @@
       <c r="A35" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -727,10 +745,10 @@
       <c r="A36" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="1" t="s">
+      <c r="B36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -738,10 +756,10 @@
       <c r="A37" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -749,10 +767,10 @@
       <c r="A38" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -760,7 +778,7 @@
       <c r="B39" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -771,7 +789,7 @@
       <c r="B40" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C40" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -779,10 +797,10 @@
       <c r="A41" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" s="1" t="s">
+      <c r="B41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -790,18 +808,18 @@
       <c r="A42" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C43" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -809,10 +827,10 @@
       <c r="A44" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -820,10 +838,10 @@
       <c r="A45" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -842,10 +860,10 @@
       <c r="A47" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C47" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -856,7 +874,7 @@
       <c r="B48" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -864,7 +882,7 @@
       <c r="B49" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -875,7 +893,7 @@
       <c r="B50" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>56</v>
       </c>
     </row>
@@ -883,7 +901,7 @@
       <c r="A51" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="0" t="s">
@@ -891,7 +909,7 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C52" s="0" t="s">
@@ -921,7 +939,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C55" s="0" t="s">
@@ -932,7 +950,7 @@
       <c r="A56" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C56" s="0" t="s">
@@ -943,10 +961,10 @@
       <c r="A57" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C57" s="1" t="s">
+      <c r="B57" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -954,10 +972,10 @@
       <c r="A58" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C58" s="2" t="s">
         <v>68</v>
       </c>
     </row>
@@ -965,18 +983,18 @@
       <c r="A59" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C59" s="1" t="s">
+      <c r="C59" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="1" t="s">
+      <c r="C60" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -984,10 +1002,10 @@
       <c r="A61" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C61" s="1" t="s">
+      <c r="C61" s="2" t="s">
         <v>71</v>
       </c>
     </row>
@@ -995,10 +1013,10 @@
       <c r="A62" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C62" s="1" t="s">
+      <c r="B62" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1006,10 +1024,10 @@
       <c r="A63" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C63" s="1" t="s">
+      <c r="C63" s="2" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>